<commit_message>
update license tables and added treemap chart
</commit_message>
<xml_diff>
--- a/output/licenses_2020_processed_AI.xlsx
+++ b/output/licenses_2020_processed_AI.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="113" documentId="11_E88293383C096B40D363319A961B185C02DA4E0A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C54E18CB-1292-41C7-AFA4-91CE636C65C1}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/jan_taubitz_charite_de/Documents/_BIH/BUA-Dashboards/fair-assessment/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="114" documentId="11_E88293383C096B40D363319A961B185C02DA4E0A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{000511DD-6A26-4076-9450-029A76D498F6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="licenses_2020_processed_AI" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2512" uniqueCount="695">
   <si>
     <t>article</t>
   </si>
@@ -2111,13 +2116,16 @@
   </si>
   <si>
     <t>http://doi.org/10.2210/pdb6Z9P/pdb</t>
+  </si>
+  <si>
+    <t>True für FAIR-Enough! CC BY-NC-ND, metadata file!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2157,20 +2165,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2467,13 +2478,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="D294" sqref="D294"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2511,7 +2522,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2549,7 +2560,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -2587,14 +2598,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="255">
+    <row r="4" spans="1:12" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D4" t="s">
@@ -2625,7 +2636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -2663,7 +2674,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -2698,7 +2709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2730,7 +2741,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2762,7 +2773,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -2794,7 +2805,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2826,7 +2837,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2858,7 +2869,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -2890,7 +2901,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -2922,7 +2933,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -2954,7 +2965,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -2986,7 +2997,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -3018,7 +3029,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -3050,7 +3061,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -3082,7 +3093,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -3114,7 +3125,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -3146,7 +3157,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -3178,7 +3189,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -3210,7 +3221,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>83</v>
       </c>
@@ -3242,7 +3253,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -3274,7 +3285,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>87</v>
       </c>
@@ -3306,7 +3317,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -3338,7 +3349,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -3370,7 +3381,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -3402,7 +3413,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -3434,7 +3445,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -3466,7 +3477,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>101</v>
       </c>
@@ -3498,7 +3509,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -3530,7 +3541,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -3562,7 +3573,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -3594,7 +3605,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -3626,7 +3637,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>112</v>
       </c>
@@ -3658,7 +3669,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -3690,7 +3701,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>118</v>
       </c>
@@ -3722,7 +3733,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>123</v>
       </c>
@@ -3754,7 +3765,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>125</v>
       </c>
@@ -3786,7 +3797,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>127</v>
       </c>
@@ -3818,7 +3829,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>129</v>
       </c>
@@ -3850,7 +3861,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>131</v>
       </c>
@@ -3882,7 +3893,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>133</v>
       </c>
@@ -3914,7 +3925,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>135</v>
       </c>
@@ -3946,7 +3957,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -3978,7 +3989,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>139</v>
       </c>
@@ -4016,14 +4027,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>145</v>
       </c>
       <c r="B48" t="s">
         <v>146</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D48" t="s">
@@ -4048,7 +4059,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>151</v>
       </c>
@@ -4080,7 +4091,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>154</v>
       </c>
@@ -4112,7 +4123,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>156</v>
       </c>
@@ -4144,7 +4155,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>158</v>
       </c>
@@ -4176,7 +4187,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>160</v>
       </c>
@@ -4208,7 +4219,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>162</v>
       </c>
@@ -4240,14 +4251,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="180">
+    <row r="55" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>164</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="4" t="s">
         <v>165</v>
       </c>
       <c r="D55" t="s">
@@ -4278,7 +4289,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>171</v>
       </c>
@@ -4310,7 +4321,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>174</v>
       </c>
@@ -4342,7 +4353,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>177</v>
       </c>
@@ -4374,14 +4385,14 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>179</v>
       </c>
       <c r="B59" t="s">
         <v>180</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="4" t="s">
         <v>180</v>
       </c>
       <c r="D59" t="s">
@@ -4406,7 +4417,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -4438,7 +4449,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>182</v>
       </c>
@@ -4470,7 +4481,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>184</v>
       </c>
@@ -4502,7 +4513,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>187</v>
       </c>
@@ -4534,7 +4545,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>189</v>
       </c>
@@ -4566,7 +4577,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>191</v>
       </c>
@@ -4598,7 +4609,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>193</v>
       </c>
@@ -4630,7 +4641,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>195</v>
       </c>
@@ -4662,7 +4673,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>198</v>
       </c>
@@ -4694,7 +4705,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>200</v>
       </c>
@@ -4726,7 +4737,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>202</v>
       </c>
@@ -4758,7 +4769,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>204</v>
       </c>
@@ -4790,7 +4801,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -4822,7 +4833,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>208</v>
       </c>
@@ -4854,7 +4865,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>210</v>
       </c>
@@ -4886,7 +4897,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>212</v>
       </c>
@@ -4918,7 +4929,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>214</v>
       </c>
@@ -4956,7 +4967,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>220</v>
       </c>
@@ -4991,7 +5002,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>226</v>
       </c>
@@ -5023,7 +5034,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>228</v>
       </c>
@@ -5055,7 +5066,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>230</v>
       </c>
@@ -5087,7 +5098,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>232</v>
       </c>
@@ -5119,7 +5130,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>234</v>
       </c>
@@ -5151,7 +5162,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>236</v>
       </c>
@@ -5183,7 +5194,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>135</v>
       </c>
@@ -5215,7 +5226,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>243</v>
       </c>
@@ -5247,7 +5258,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>248</v>
       </c>
@@ -5279,7 +5290,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>250</v>
       </c>
@@ -5311,7 +5322,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>252</v>
       </c>
@@ -5343,7 +5354,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>254</v>
       </c>
@@ -5375,7 +5386,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>256</v>
       </c>
@@ -5407,7 +5418,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>258</v>
       </c>
@@ -5439,7 +5450,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>260</v>
       </c>
@@ -5471,7 +5482,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>262</v>
       </c>
@@ -5503,7 +5514,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>267</v>
       </c>
@@ -5535,7 +5546,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>269</v>
       </c>
@@ -5567,7 +5578,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>271</v>
       </c>
@@ -5599,7 +5610,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>273</v>
       </c>
@@ -5631,7 +5642,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>275</v>
       </c>
@@ -5663,7 +5674,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>277</v>
       </c>
@@ -5695,7 +5706,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>278</v>
       </c>
@@ -5727,7 +5738,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>282</v>
       </c>
@@ -5759,7 +5770,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>287</v>
       </c>
@@ -5794,14 +5805,14 @@
         <v>292</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>154</v>
       </c>
       <c r="B103" t="s">
         <v>293</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="4" t="s">
         <v>293</v>
       </c>
       <c r="D103" t="s">
@@ -5820,16 +5831,16 @@
         <v>295</v>
       </c>
       <c r="I103" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="J103" t="s">
-        <v>291</v>
+        <v>694</v>
       </c>
       <c r="K103" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>184</v>
       </c>
@@ -5861,7 +5872,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>299</v>
       </c>
@@ -5893,7 +5904,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>303</v>
       </c>
@@ -5925,7 +5936,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>304</v>
       </c>
@@ -5957,7 +5968,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>305</v>
       </c>
@@ -5989,7 +6000,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>307</v>
       </c>
@@ -6021,7 +6032,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>308</v>
       </c>
@@ -6053,7 +6064,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>310</v>
       </c>
@@ -6085,7 +6096,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>311</v>
       </c>
@@ -6117,7 +6128,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>314</v>
       </c>
@@ -6149,7 +6160,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>319</v>
       </c>
@@ -6181,7 +6192,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>321</v>
       </c>
@@ -6213,7 +6224,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>323</v>
       </c>
@@ -6245,7 +6256,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>325</v>
       </c>
@@ -6277,7 +6288,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>327</v>
       </c>
@@ -6309,7 +6320,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>329</v>
       </c>
@@ -6341,7 +6352,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>331</v>
       </c>
@@ -6373,7 +6384,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>333</v>
       </c>
@@ -6405,7 +6416,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>335</v>
       </c>
@@ -6437,7 +6448,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>337</v>
       </c>
@@ -6469,7 +6480,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>339</v>
       </c>
@@ -6501,7 +6512,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>341</v>
       </c>
@@ -6533,7 +6544,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>343</v>
       </c>
@@ -6565,7 +6576,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>345</v>
       </c>
@@ -6597,7 +6608,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>347</v>
       </c>
@@ -6629,7 +6640,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>349</v>
       </c>
@@ -6661,7 +6672,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>299</v>
       </c>
@@ -6693,7 +6704,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>355</v>
       </c>
@@ -6725,7 +6736,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>357</v>
       </c>
@@ -6757,7 +6768,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>359</v>
       </c>
@@ -6789,7 +6800,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>361</v>
       </c>
@@ -6821,7 +6832,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>363</v>
       </c>
@@ -6853,7 +6864,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>365</v>
       </c>
@@ -6885,7 +6896,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>367</v>
       </c>
@@ -6917,7 +6928,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>369</v>
       </c>
@@ -6949,7 +6960,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>371</v>
       </c>
@@ -6981,7 +6992,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>373</v>
       </c>
@@ -7013,7 +7024,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>375</v>
       </c>
@@ -7045,7 +7056,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>377</v>
       </c>
@@ -7077,7 +7088,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>379</v>
       </c>
@@ -7109,7 +7120,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>381</v>
       </c>
@@ -7141,7 +7152,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>329</v>
       </c>
@@ -7173,7 +7184,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>384</v>
       </c>
@@ -7205,7 +7216,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>386</v>
       </c>
@@ -7237,7 +7248,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>388</v>
       </c>
@@ -7269,7 +7280,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>390</v>
       </c>
@@ -7301,7 +7312,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>392</v>
       </c>
@@ -7333,7 +7344,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>394</v>
       </c>
@@ -7365,7 +7376,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>396</v>
       </c>
@@ -7397,7 +7408,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>398</v>
       </c>
@@ -7429,7 +7440,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>214</v>
       </c>
@@ -7461,7 +7472,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>401</v>
       </c>
@@ -7493,7 +7504,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>403</v>
       </c>
@@ -7525,7 +7536,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>405</v>
       </c>
@@ -7557,7 +7568,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>407</v>
       </c>
@@ -7589,7 +7600,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -7621,7 +7632,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>410</v>
       </c>
@@ -7653,7 +7664,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>412</v>
       </c>
@@ -7685,7 +7696,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>414</v>
       </c>
@@ -7717,7 +7728,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>416</v>
       </c>
@@ -7749,7 +7760,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>418</v>
       </c>
@@ -7781,7 +7792,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>420</v>
       </c>
@@ -7813,7 +7824,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>422</v>
       </c>
@@ -7845,7 +7856,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>424</v>
       </c>
@@ -7877,7 +7888,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>426</v>
       </c>
@@ -7909,7 +7920,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>428</v>
       </c>
@@ -7941,7 +7952,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>252</v>
       </c>
@@ -7973,7 +7984,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>431</v>
       </c>
@@ -8005,7 +8016,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>433</v>
       </c>
@@ -8037,7 +8048,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>435</v>
       </c>
@@ -8069,7 +8080,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>437</v>
       </c>
@@ -8101,7 +8112,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>439</v>
       </c>
@@ -8133,7 +8144,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>441</v>
       </c>
@@ -8165,7 +8176,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>443</v>
       </c>
@@ -8197,7 +8208,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>445</v>
       </c>
@@ -8229,7 +8240,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>446</v>
       </c>
@@ -8261,7 +8272,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>448</v>
       </c>
@@ -8293,7 +8304,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>450</v>
       </c>
@@ -8325,7 +8336,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>452</v>
       </c>
@@ -8357,7 +8368,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>454</v>
       </c>
@@ -8389,7 +8400,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>456</v>
       </c>
@@ -8421,7 +8432,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>458</v>
       </c>
@@ -8453,7 +8464,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>460</v>
       </c>
@@ -8485,7 +8496,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>462</v>
       </c>
@@ -8517,7 +8528,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>464</v>
       </c>
@@ -8549,7 +8560,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>466</v>
       </c>
@@ -8581,7 +8592,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>468</v>
       </c>
@@ -8613,7 +8624,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>470</v>
       </c>
@@ -8645,7 +8656,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>472</v>
       </c>
@@ -8677,7 +8688,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>474</v>
       </c>
@@ -8709,7 +8720,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>476</v>
       </c>
@@ -8741,7 +8752,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>478</v>
       </c>
@@ -8773,7 +8784,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>341</v>
       </c>
@@ -8805,7 +8816,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>480</v>
       </c>
@@ -8837,7 +8848,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>482</v>
       </c>
@@ -8869,7 +8880,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>484</v>
       </c>
@@ -8901,7 +8912,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>486</v>
       </c>
@@ -8933,7 +8944,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>488</v>
       </c>
@@ -8965,7 +8976,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>490</v>
       </c>
@@ -8997,7 +9008,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>492</v>
       </c>
@@ -9029,7 +9040,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>494</v>
       </c>
@@ -9061,7 +9072,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>496</v>
       </c>
@@ -9093,7 +9104,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>498</v>
       </c>
@@ -9125,7 +9136,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>500</v>
       </c>
@@ -9157,7 +9168,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>502</v>
       </c>
@@ -9189,7 +9200,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="209" spans="1:11">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>504</v>
       </c>
@@ -9221,7 +9232,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="210" spans="1:11">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>506</v>
       </c>
@@ -9253,7 +9264,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="211" spans="1:11">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>508</v>
       </c>
@@ -9285,7 +9296,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="212" spans="1:11">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>510</v>
       </c>
@@ -9317,7 +9328,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="213" spans="1:11">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>512</v>
       </c>
@@ -9349,7 +9360,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="214" spans="1:11">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>514</v>
       </c>
@@ -9381,7 +9392,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="215" spans="1:11">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>516</v>
       </c>
@@ -9413,7 +9424,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>518</v>
       </c>
@@ -9445,7 +9456,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="217" spans="1:11">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>520</v>
       </c>
@@ -9477,7 +9488,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>171</v>
       </c>
@@ -9509,7 +9520,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="219" spans="1:11">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>526</v>
       </c>
@@ -9541,7 +9552,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>530</v>
       </c>
@@ -9573,14 +9584,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="221" spans="1:11">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>532</v>
       </c>
       <c r="B221" t="s">
         <v>533</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C221" s="4" t="s">
         <v>533</v>
       </c>
       <c r="D221" t="s">
@@ -9605,7 +9616,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>536</v>
       </c>
@@ -9640,7 +9651,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="223" spans="1:11">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>542</v>
       </c>
@@ -9672,7 +9683,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="224" spans="1:11">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>547</v>
       </c>
@@ -9704,7 +9715,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>550</v>
       </c>
@@ -9736,7 +9747,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>262</v>
       </c>
@@ -9768,7 +9779,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>39</v>
       </c>
@@ -9800,7 +9811,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>557</v>
       </c>
@@ -9832,7 +9843,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>559</v>
       </c>
@@ -9864,7 +9875,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>273</v>
       </c>
@@ -9896,7 +9907,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>325</v>
       </c>
@@ -9928,7 +9939,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>154</v>
       </c>
@@ -9960,7 +9971,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>564</v>
       </c>
@@ -9992,7 +10003,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>566</v>
       </c>
@@ -10024,7 +10035,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>568</v>
       </c>
@@ -10056,7 +10067,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>570</v>
       </c>
@@ -10088,7 +10099,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>572</v>
       </c>
@@ -10120,7 +10131,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>496</v>
       </c>
@@ -10152,7 +10163,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>575</v>
       </c>
@@ -10184,7 +10195,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>577</v>
       </c>
@@ -10216,7 +10227,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="241" spans="1:11">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>133</v>
       </c>
@@ -10251,7 +10262,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="242" spans="1:11">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>133</v>
       </c>
@@ -10283,7 +10294,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>267</v>
       </c>
@@ -10315,7 +10326,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>277</v>
       </c>
@@ -10347,7 +10358,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="245" spans="1:11">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>588</v>
       </c>
@@ -10379,14 +10390,14 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="246" spans="1:11">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>590</v>
       </c>
       <c r="B246" t="s">
         <v>591</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C246" s="4" t="s">
         <v>592</v>
       </c>
       <c r="D246" t="s">
@@ -10411,7 +10422,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>594</v>
       </c>
@@ -10443,7 +10454,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>597</v>
       </c>
@@ -10475,7 +10486,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>267</v>
       </c>
@@ -10507,7 +10518,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>602</v>
       </c>
@@ -10539,7 +10550,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="251" spans="1:11">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>321</v>
       </c>
@@ -10571,7 +10582,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="252" spans="1:11">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>277</v>
       </c>
@@ -10603,7 +10614,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="253" spans="1:11">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>365</v>
       </c>
@@ -10635,7 +10646,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="254" spans="1:11">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>384</v>
       </c>
@@ -10667,7 +10678,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="255" spans="1:11">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>401</v>
       </c>
@@ -10699,7 +10710,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="256" spans="1:11">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>609</v>
       </c>
@@ -10731,7 +10742,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>611</v>
       </c>
@@ -10763,7 +10774,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>613</v>
       </c>
@@ -10795,7 +10806,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>81</v>
       </c>
@@ -10827,7 +10838,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>616</v>
       </c>
@@ -10859,7 +10870,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>618</v>
       </c>
@@ -10891,7 +10902,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>620</v>
       </c>
@@ -10923,7 +10934,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>437</v>
       </c>
@@ -10955,7 +10966,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>158</v>
       </c>
@@ -10987,7 +10998,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>624</v>
       </c>
@@ -11019,7 +11030,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>626</v>
       </c>
@@ -11051,7 +11062,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>488</v>
       </c>
@@ -11083,7 +11094,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>629</v>
       </c>
@@ -11115,7 +11126,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>631</v>
       </c>
@@ -11147,7 +11158,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>331</v>
       </c>
@@ -11179,7 +11190,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>635</v>
       </c>
@@ -11211,7 +11222,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>638</v>
       </c>
@@ -11243,7 +11254,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>640</v>
       </c>
@@ -11275,7 +11286,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>642</v>
       </c>
@@ -11307,7 +11318,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>644</v>
       </c>
@@ -11339,7 +11350,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>646</v>
       </c>
@@ -11371,7 +11382,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>647</v>
       </c>
@@ -11403,7 +11414,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>649</v>
       </c>
@@ -11435,7 +11446,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>651</v>
       </c>
@@ -11467,7 +11478,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>433</v>
       </c>
@@ -11499,7 +11510,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>654</v>
       </c>
@@ -11531,7 +11542,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>656</v>
       </c>
@@ -11563,7 +11574,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>658</v>
       </c>
@@ -11595,7 +11606,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>299</v>
       </c>
@@ -11627,7 +11638,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>662</v>
       </c>
@@ -11659,7 +11670,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>663</v>
       </c>
@@ -11691,7 +11702,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>665</v>
       </c>
@@ -11723,7 +11734,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>669</v>
       </c>
@@ -11755,7 +11766,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>671</v>
       </c>
@@ -11787,7 +11798,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>673</v>
       </c>
@@ -11819,7 +11830,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>151</v>
       </c>
@@ -11851,7 +11862,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>662</v>
       </c>
@@ -11883,7 +11894,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>256</v>
       </c>
@@ -11915,7 +11926,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>679</v>
       </c>
@@ -11947,7 +11958,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>682</v>
       </c>
@@ -11979,7 +11990,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>684</v>
       </c>
@@ -12011,7 +12022,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="297" spans="1:10">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>154</v>
       </c>
@@ -12043,7 +12054,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>665</v>
       </c>
@@ -12075,7 +12086,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>669</v>
       </c>
@@ -12107,7 +12118,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>689</v>
       </c>
@@ -12139,7 +12150,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>691</v>
       </c>
@@ -12171,7 +12182,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="302" spans="1:10">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>673</v>
       </c>
@@ -12205,30 +12216,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{0416EBC3-8D8D-481F-8AE5-4EE303E3A61A}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{3D158592-DBDD-4E7C-80E8-EC7550D49540}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{94EE5BAB-7F14-43C5-A28B-7F456B55B6B0}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{0F27C323-B0AB-4F41-AA5A-333DCD771D2F}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{A006C341-A7EC-47B0-AC64-C3C6F2C68252}"/>
-    <hyperlink ref="B6" r:id="rId6" xr:uid="{D3169253-9DF3-4968-95FC-A177AC122101}"/>
-    <hyperlink ref="B47" r:id="rId7" xr:uid="{91DC6AE2-0799-4F2A-8C41-944E0088A668}"/>
-    <hyperlink ref="B55" r:id="rId8" xr:uid="{AC4E8A00-1C31-4C02-8BEB-1C91090ED3CB}"/>
-    <hyperlink ref="B76" r:id="rId9" xr:uid="{7A76082B-9939-45D7-84DD-1483F1134A10}"/>
-    <hyperlink ref="B77" r:id="rId10" xr:uid="{25C8F280-2106-49E7-A00E-EC7247FF32D3}"/>
-    <hyperlink ref="C77" r:id="rId11" xr:uid="{311A40A2-52D8-4648-BD02-A355B771BA9E}"/>
-    <hyperlink ref="B84" r:id="rId12" xr:uid="{3612D7D8-F06D-40BB-946D-8792C56EEB1F}"/>
-    <hyperlink ref="B100" r:id="rId13" xr:uid="{C35BE4DB-F34B-4DD0-AF54-79134BFDC938}"/>
-    <hyperlink ref="C102" r:id="rId14" xr:uid="{0E9DA7FD-567A-46BE-A2D7-10793AF62C16}"/>
-    <hyperlink ref="B218" r:id="rId15" xr:uid="{A07E9204-AEA5-4365-8A9C-9E8DC2E4653F}"/>
-    <hyperlink ref="B222" r:id="rId16" xr:uid="{9C138A55-4B7B-42E5-BC75-59FC81EAF11E}"/>
-    <hyperlink ref="B225" r:id="rId17" xr:uid="{E68C9F93-F9EC-4E95-A11B-D60DCE981862}"/>
-    <hyperlink ref="B241" r:id="rId18" xr:uid="{0604709A-D485-49E7-8D5D-35AA4EEC6772}"/>
-    <hyperlink ref="C48" r:id="rId19" xr:uid="{C32D950A-6E6A-426E-9B80-525230F9C044}"/>
-    <hyperlink ref="B291" r:id="rId20" xr:uid="{88ECB2FA-9CD5-4896-A7D3-4AB033937DC8}"/>
-    <hyperlink ref="B248" r:id="rId21" xr:uid="{DEDEF606-109A-4F1B-9C9D-D67514E8CF3B}"/>
-    <hyperlink ref="C288" r:id="rId22" xr:uid="{630AB60C-DEC6-47CA-B2C3-F635F5062897}"/>
-    <hyperlink ref="C114" r:id="rId23" xr:uid="{91F2D16C-99E8-4A56-A1FD-D7791AE56949}"/>
-    <hyperlink ref="B224" r:id="rId24" location="%7B%22table_sort_history%22%3A%22main.collection_asc%22%7D" xr:uid="{6B1689BF-02BE-41DB-A636-D1DF14D3FB29}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{44EBB43D-8A42-4324-B7B6-7195C6A87FF4}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{02508A53-5A50-4665-8640-1ED923F3B01A}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{774C51FE-9751-46B8-8034-C73DBAB5A203}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{867BF276-AA8C-497E-BBA5-DFD7C2D83833}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{869C2789-E044-49CD-8131-D19BF2886331}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{45F76C5B-A6F6-477C-B95F-A44F75BBEF28}"/>
+    <hyperlink ref="B47" r:id="rId7" xr:uid="{D49236E5-4485-4DEE-B647-ED6CAF3FE824}"/>
+    <hyperlink ref="B55" r:id="rId8" xr:uid="{E880B654-D6D3-4549-965F-22B2658F180B}"/>
+    <hyperlink ref="B76" r:id="rId9" xr:uid="{08C51FA7-9A8D-4D58-9EC1-D3D639112017}"/>
+    <hyperlink ref="B77" r:id="rId10" xr:uid="{70FE3AC0-5E4F-4A6C-BEF0-13BD97B84A46}"/>
+    <hyperlink ref="C77" r:id="rId11" xr:uid="{FB6DC53C-2972-4235-BCD7-40BBFD206E7E}"/>
+    <hyperlink ref="B84" r:id="rId12" xr:uid="{9D934CB7-E4C6-4B48-BE37-218C353B8DEE}"/>
+    <hyperlink ref="B100" r:id="rId13" xr:uid="{8F676046-E817-40E9-A9CB-915810335400}"/>
+    <hyperlink ref="C102" r:id="rId14" xr:uid="{4F45DBE9-967D-427F-BBC3-AD3142D5D1E2}"/>
+    <hyperlink ref="B218" r:id="rId15" xr:uid="{99C87AAB-2C19-4FC7-9114-71BFF39CA264}"/>
+    <hyperlink ref="B222" r:id="rId16" xr:uid="{2E326331-7E14-4CEB-9168-6DBE171D4A2E}"/>
+    <hyperlink ref="B225" r:id="rId17" xr:uid="{59C28CF3-BC57-4280-ABEE-3DFD267BE5AC}"/>
+    <hyperlink ref="B241" r:id="rId18" xr:uid="{D0692A8D-9BBC-45CE-B436-2A60C49FABE1}"/>
+    <hyperlink ref="C48" r:id="rId19" xr:uid="{5FCB6E05-004E-4235-9CEB-A32A99F31F3E}"/>
+    <hyperlink ref="B291" r:id="rId20" xr:uid="{7503AD8A-C44C-4083-A81D-911F42317A09}"/>
+    <hyperlink ref="B248" r:id="rId21" xr:uid="{2BC16F65-F2F0-41F3-B41E-179C5CF6B0B5}"/>
+    <hyperlink ref="C288" r:id="rId22" xr:uid="{69705EFD-0F27-418D-AB9D-57E0FA7091F2}"/>
+    <hyperlink ref="C114" r:id="rId23" xr:uid="{02FBF733-B8D7-48DB-969D-B47F62E38101}"/>
+    <hyperlink ref="B224" r:id="rId24" location="%7B%22table_sort_history%22%3A%22main.collection_asc%22%7D" xr:uid="{A0C88139-DADF-4F60-AC03-3808CADC560E}"/>
+    <hyperlink ref="C55" r:id="rId25" xr:uid="{A2A29B9D-530F-4893-961F-ADCE43487F7B}"/>
+    <hyperlink ref="C59" r:id="rId26" xr:uid="{FA29D142-268D-4BCC-987A-9682029E1764}"/>
+    <hyperlink ref="C103" r:id="rId27" xr:uid="{733E2954-10AA-4497-964C-AD3A913CD55B}"/>
+    <hyperlink ref="C246" r:id="rId28" xr:uid="{28B08CCA-43E5-4C49-80F3-5335136BBBF6}"/>
+    <hyperlink ref="C221" r:id="rId29" xr:uid="{CDD78531-94C2-4D65-B861-F8675E3C5040}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>